<commit_message>
first try attention DG
</commit_message>
<xml_diff>
--- a/results_dGAN_torchdGAN.xlsx
+++ b/results_dGAN_torchdGAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Python Scripts\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Python Scripts\MA\torchDoppelGANger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2C0DF7-0FE3-40EF-914A-A1141CF47F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCC2859-F785-4EA4-A338-830759D8E8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{72B96DE4-1843-45BE-9EB3-3139DDEC3D33}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{72B96DE4-1843-45BE-9EB3-3139DDEC3D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="81">
   <si>
     <t>Structural Characterization</t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>need other GANs for comparison</t>
+  </si>
+  <si>
+    <t>MSE_AUTOCORRELATION</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -690,6 +693,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1248,6 +1255,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1512252</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>125411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>30796</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>136571</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB796535-E392-42E4-801D-A61D494244AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1512252" y="2176461"/>
+          <a:ext cx="2912744" cy="2036810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1752,7 +1808,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B06D56-6B93-4A2B-B49E-4D8F83BF7FE8}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1936,13 +1994,188 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21BB0B33-48FD-4F84-A7A3-3188F47B44E2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="39"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1950,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B6C292-0951-4FED-B31A-918410177566}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2514,9 +2747,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473216AF-082B-4ACC-A583-07433FC63B89}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:J11"/>
+      <selection pane="topRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2585,9 +2818,9 @@
       <c r="A3" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="47"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="15"/>
       <c r="F3" s="46"/>
       <c r="G3" s="16"/>

</xml_diff>